<commit_message>
check out of range
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="42">
   <si>
     <t>序号</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
   <si>
     <t>aafffffffffffffffffffffffffffffffff</t>
@@ -1408,7 +1411,7 @@
   <dimension ref="A3:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I6" sqref="I6:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1452,7 +1455,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1476,6 +1479,9 @@
       </c>
       <c r="I4" t="s">
         <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1486,22 +1492,22 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1509,22 +1515,22 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1532,22 +1538,22 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1555,45 +1561,49 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1601,22 +1611,22 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1624,22 +1634,22 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1647,22 +1657,22 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
         <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1670,22 +1680,22 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1693,22 +1703,22 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1716,22 +1726,22 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
         <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1739,22 +1749,22 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1762,22 +1772,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s">
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1785,22 +1795,22 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s">
         <v>15</v>
       </c>
       <c r="H18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1808,22 +1818,22 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G19" t="s">
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1831,22 +1841,22 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
         <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1854,7 +1864,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>11</v>
@@ -1863,13 +1873,13 @@
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G21" t="s">
         <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I21" t="s">
         <v>17</v>
@@ -1895,12 +1905,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>